<commit_message>
Started CLR for test ingest
</commit_message>
<xml_diff>
--- a/bangarang/CLR/CLR_bangarang.xlsx
+++ b/bangarang/CLR/CLR_bangarang.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="648">
   <si>
     <t>text</t>
   </si>
@@ -2077,8 +2077,76 @@
     <t>Picard, Chris R.</t>
   </si>
   <si>
-    <t>Public Data Collection of the "Bangarang Project", the dissertation project of Eric Keen at Scripps Institution of Oceanography. These data are used in multiple chapters of that dissertation as well as their corresponding peer-reviewed publications. More information about this research can be found at its website: &lt;a href="www.rvbangarang.org"&gt;www.rvbangarang.org&lt;/a&gt;.
+    <t>data | text</t>
+  </si>
+  <si>
+    <t>Kitimat Fjord System</t>
+  </si>
+  <si>
+    <t>Humpback whale | Gitga'at First Nation | Fin whale</t>
+  </si>
+  <si>
+    <t>Tail_no_bg.jpg</t>
+  </si>
+  <si>
+    <t>Public Data Collection of the "Bangarang Project", the dissertation project of Eric Keen at Scripps Institution of Oceanography. These data are used in multiple chapters of that dissertation as well as their corresponding peer-reviewed publications. More information about this research can be found at its website: &lt;a href="https://rvbangarang.org/"&gt;rvbangarang.org&lt;/a&gt;.
 Metadata were prepared by Eric Keen, &lt;a href="mailto:ekeen@ucsd.edu"&gt;ekeen@ucsd.edu&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Data associated with the "Bangarang Project", Eric Keen's dissertation study on the foraging ecology of whales in the Kitimat Fjord System, British Columbia.</t>
+  </si>
+  <si>
+    <t>Bangarang Site @ https://rvbangarang.org/</t>
+  </si>
+  <si>
+    <t>2013_x000D_
+National Geographic Society Waitt Grant (Grant number 2681-13)_x000D_
+Mullin Award from the Biological Oceanography group at Scripps Institution of Oceanography (SIO)_x000D_
+2012 NSF Graduate Research Fellowship (GRF) video contest._x000D_
+DFO Cetacean Research Program_x000D_
+_x000D_
+2014_x000D_
+Gitga’at Guardian Watchmen Program_x000D_
+Explorers Club Exploration Fund_x000D_
+Cascadia Research Collective_x000D_
+Scripps Institution of Oceanography Department (thanks in particular to Maureen McGreevey and Denise Darling)_x000D_
+DFO Cetacean Research Program_x000D_
+_x000D_
+Engine Rebuild Donors:_x000D_
+The Cunningham Foundation (Joel and Trudy)_x000D_
+Robert and Patricia Ayres_x000D_
+Jim Watson_x000D_
+Jay Barlow and Barb Taylor_x000D_
+_x000D_
+Crowd-sourcing donors:_x000D_
+Bill Wood and Kathy Wood-Dobbins_x000D_
+Rhonda Keen_x000D_
+Mary and Norm Humber_x000D_
+Klaus Wilging_x000D_
+_x000D_
+2015_x000D_
+Gitga’at Guardian Watchmen Program_x000D_
+Lewis and Clark Fund, American Philosophical Society_x000D_
+Cascadia Research Collective_x000D_
+Office of Naval Research and SIO Whale Acoustics Lab_x000D_
+_x000D_
+Private supporters:_x000D_
+Jim Watson_x000D_
+Robert and Patricia Ayres</t>
+  </si>
+  <si>
+    <t>Keen, EM. (In Preparation) Habitat use strategies of sympatric rorqual whales within a fjord system: what does “critical habitat” mean for mobile marine predators? Doctoral Thesis. University of California: San Diego._x000D_
+_x000D_
+Keen, EM, et al. (In Review) From fjord to fin: dive energetics link ocean features to competitive dynamics in sympatric rorqual whales. PLOS ONE._x000D_
+_x000D_
+Keen, EM, KM Qualls, KL Thompson, J Wray, CR Picard. (In Review) Novel spatial analytics to identify candidate environmental cues for foraging whales. Biology Letters._x000D_
+_x000D_
+Keen, EM, et al.. (In Review) Parsing habitat use strategies of sympatric rorquals whales within a fjord system. Canadian Journal of Zoology._x000D_
+_x000D_
+Keen, EM. (In Review) Aggregative and feeding thresholds of sympatric rorqual whales within a fjord system. Ecosphere.</t>
+  </si>
+  <si>
+    <t>Megaptera novaeangliae | Balaenoptera physalus</t>
   </si>
 </sst>
 </file>
@@ -3121,39 +3189,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="23.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="22" style="3" customWidth="1"/>
     <col min="5" max="5" width="51.5703125" style="3" customWidth="1"/>
     <col min="6" max="8" width="45.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="45.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="57.28515625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="39.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="42.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="44.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="84.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" style="3" customWidth="1"/>
+    <col min="13" max="15" width="57.28515625" style="3" customWidth="1"/>
+    <col min="16" max="18" width="42.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>621</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -3187,22 +3252,34 @@
         <v>3</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>519</v>
+        <v>628</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>520</v>
+        <v>629</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>521</v>
+        <v>454</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>638</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>357</v>
       </c>
@@ -3227,8 +3304,29 @@
       <c r="K2" s="3" t="s">
         <v>635</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>643</v>
+      </c>
       <c r="M2" s="3" t="s">
-        <v>638</v>
+        <v>642</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -3240,13 +3338,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
-          <x14:formula1>
-            <xm:f>'CV values'!$C$2:$C$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -3269,19 +3361,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>O1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>P1</xm:sqref>
+          <xm:sqref>P1:R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Q1</xm:sqref>
+          <xm:sqref>S1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3293,13 +3379,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>N1</xm:sqref>
+          <xm:sqref>M1:O1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added citations and changed technical note based on QA report
</commit_message>
<xml_diff>
--- a/bangarang/CLR/CLR_bangarang.xlsx
+++ b/bangarang/CLR/CLR_bangarang.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="649">
   <si>
     <t>text</t>
   </si>
@@ -2147,6 +2147,9 @@
   </si>
   <si>
     <t>Megaptera novaeangliae | Balaenoptera physalus</t>
+  </si>
+  <si>
+    <t>Keen, Eric M. (2017): The Bangarang Project. UC San Diego Library Digital Collections. http://doi.org/10.6075/J0MK69TN</t>
   </si>
 </sst>
 </file>
@@ -3189,10 +3192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,12 +3209,12 @@
     <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="32.28515625" style="3" customWidth="1"/>
-    <col min="13" max="15" width="57.28515625" style="3" customWidth="1"/>
-    <col min="16" max="18" width="42.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="84.28515625" style="3" customWidth="1"/>
+    <col min="13" max="16" width="57.28515625" style="3" customWidth="1"/>
+    <col min="17" max="19" width="42.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3252,25 +3255,28 @@
         <v>3</v>
       </c>
       <c r="N1" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>629</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>509</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>459</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
@@ -3311,21 +3317,24 @@
         <v>642</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>644</v>
       </c>
     </row>
@@ -3361,13 +3370,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>P1:R1</xm:sqref>
+          <xm:sqref>Q1:S1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>S1</xm:sqref>
+          <xm:sqref>T1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3379,7 +3388,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:O1</xm:sqref>
+          <xm:sqref>M1:P1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>